<commit_message>
Uncomment kill 1C app
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\RPA\1C_pay_petrol\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B8611E-9F41-409D-AB6F-D1106C4CE0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCA5132-E62C-4420-83C7-72C853F39C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="4005" windowWidth="18270" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="78">
   <si>
     <t>Name</t>
   </si>
@@ -401,9 +401,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -441,7 +441,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -547,7 +547,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -689,7 +689,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -700,7 +700,7 @@
   <dimension ref="A1:Z989"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -915,6 +915,11 @@
         <v>75</v>
       </c>
       <c r="B20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" customHeight="1">
+      <c r="B21" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>